<commit_message>
Template: Agregar opcion 'Sin informacion disponible'.
</commit_message>
<xml_diff>
--- a/backend/files/templates/template.xlsx
+++ b/backend/files/templates/template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
   <si>
     <t xml:space="preserve">Producto</t>
   </si>
@@ -47,40 +47,43 @@
     <t xml:space="preserve">Clasifición</t>
   </si>
   <si>
+    <t xml:space="preserve">Sin información disponible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importable</t>
+  </si>
+  <si>
     <t xml:space="preserve">NP001 - Frijol</t>
   </si>
   <si>
-    <t xml:space="preserve">Colones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importable</t>
+    <t xml:space="preserve">Dólares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Transable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sust. Importaciones</t>
   </si>
   <si>
     <t xml:space="preserve">NP002 - Maíz</t>
   </si>
   <si>
-    <t xml:space="preserve">Dólares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Transable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sust. Importaciones</t>
+    <t xml:space="preserve">Exportable</t>
   </si>
   <si>
     <t xml:space="preserve">NP003 - Trigo</t>
   </si>
   <si>
-    <t xml:space="preserve">Exportable</t>
+    <t xml:space="preserve">Desv. Exportaciones</t>
   </si>
   <si>
     <t xml:space="preserve">NP004 - Otros cereales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desv. Exportaciones</t>
   </si>
   <si>
     <t xml:space="preserve">NP005 - Legumbres y otras semillas oleaginosas</t>
@@ -725,10 +728,10 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -754,10 +757,6 @@
   <dataValidations count="4">
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1001" type="list">
       <formula1>Valores!$B$2:$B$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1001" type="list">
-      <formula1>Valores!$A$2:$A$185</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E1001" type="list">
@@ -766,6 +765,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1001" type="list">
       <formula1>Valores!$C$2:$C$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1001" type="list">
+      <formula1>Valores!$A$2:$A$186</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -784,13 +787,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D185"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -806,8 +809,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -820,7 +823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -834,7 +837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -842,7 +845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -850,907 +853,918 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
         <v>199</v>
       </c>
     </row>
+    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D1186" type="list">
+      <formula1>Valores!$A$2:$A$186</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>